<commit_message>
new updated data from April 24, 2025
</commit_message>
<xml_diff>
--- a/data/LS_Photonic_Processors_Updated.xlsx
+++ b/data/LS_Photonic_Processors_Updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ipronicsphotonics.sharepoint.com/sites/PaperLarge-ScalePICTrends/Documentos compartidos/paper/GitHub/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="924" documentId="13_ncr:1_{16DACA5F-4599-4788-9FE6-2FF38A319436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50787210-AA99-4299-9F00-90D978F3B635}"/>
+  <xr:revisionPtr revIDLastSave="926" documentId="13_ncr:1_{16DACA5F-4599-4788-9FE6-2FF38A319436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0D30513-52BA-42F1-BC16-C30923489E46}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8EA7BB5-C141-4C04-8AFB-6312A6445FA3}"/>
+    <workbookView minimized="1" xWindow="7200" yWindow="345" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{F8EA7BB5-C141-4C04-8AFB-6312A6445FA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Feedfoward" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Transistors" sheetId="3" r:id="rId5"/>
     <sheet name="Draft Plots" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2362" uniqueCount="917">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2364" uniqueCount="917">
   <si>
     <t>Phase shifters</t>
   </si>
@@ -29163,8 +29163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A6CAEB6-973A-4F49-9CE8-0465BE42ACE4}">
   <dimension ref="A1:AD31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P38" sqref="P38"/>
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y31" sqref="Y31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30989,6 +30989,12 @@
       </c>
       <c r="J30" s="7" t="s">
         <v>35</v>
+      </c>
+      <c r="M30" s="7" t="s">
+        <v>800</v>
+      </c>
+      <c r="V30" s="7" t="s">
+        <v>692</v>
       </c>
       <c r="AA30" t="s">
         <v>915</v>
@@ -32001,8 +32007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6A1BA7A-BF0A-46C0-890B-DAB173F75AB9}">
   <dimension ref="A1:AA29"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42978,26 +42984,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="5af84ac9-9794-49e0-853c-aa3821d89eb5" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="558e4ae2-bbe0-47dc-afec-414fd4c8278a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010029254FA996BFDD4481BAED98F366D327" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="585b57e6af3483275526db2878be4445">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="558e4ae2-bbe0-47dc-afec-414fd4c8278a" xmlns:ns3="5af84ac9-9794-49e0-853c-aa3821d89eb5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fee12902d821248c2cff660daf197e75" ns2:_="" ns3:_="">
     <xsd:import namespace="558e4ae2-bbe0-47dc-afec-414fd4c8278a"/>
@@ -43192,26 +43178,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C499E34-65D4-4959-AA67-D11E9ADE4957}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5af84ac9-9794-49e0-853c-aa3821d89eb5"/>
-    <ds:schemaRef ds:uri="558e4ae2-bbe0-47dc-afec-414fd4c8278a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1053856-28AF-4A7B-96DF-A1142500DB59}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="5af84ac9-9794-49e0-853c-aa3821d89eb5" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="558e4ae2-bbe0-47dc-afec-414fd4c8278a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2387CAC-97DE-4F89-9D07-FD40BDBFC960}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -43228,4 +43215,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1053856-28AF-4A7B-96DF-A1142500DB59}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C499E34-65D4-4959-AA67-D11E9ADE4957}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5af84ac9-9794-49e0-853c-aa3821d89eb5"/>
+    <ds:schemaRef ds:uri="558e4ae2-bbe0-47dc-afec-414fd4c8278a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>